<commit_message>
Automatische test-sync: 2025-08-18 19:45:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,8 +735,60 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Intern verzoek / Actie voor medewerker</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Bedankt, we hebben dit doorgestuurd naar support@testbedrijf123.nl.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-08-18 19:45:06</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2">
+  <conditionalFormatting sqref="D2:D3">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -756,7 +808,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2">
+  <conditionalFormatting sqref="G2:G3">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -764,17 +816,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2">
+  <conditionalFormatting sqref="H2:H3">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2">
+  <conditionalFormatting sqref="I2:I3">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2">
+  <conditionalFormatting sqref="J2:J3">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,7 +868,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 20:20:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2</f>
+              <f>'Dashboard'!$A$2:$A$3</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2</f>
+              <f>'Dashboard'!$B$2:$B$3</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,8 +787,55 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-08-18 20:20:28</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D3">
+  <conditionalFormatting sqref="D2:D4">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -808,7 +855,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G3">
+  <conditionalFormatting sqref="G2:G4">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -816,17 +863,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H3">
+  <conditionalFormatting sqref="H2:H4">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I3">
+  <conditionalFormatting sqref="I2:I4">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J3">
+  <conditionalFormatting sqref="J2:J4">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -841,7 +888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,6 +918,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 20:33:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -232,12 +232,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Dashboard'!$A$2:$A$3</f>
+              <f>'Dashboard'!$A$2:$A$4</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Dashboard'!$B$2:$B$3</f>
+              <f>'Dashboard'!$B$2:$B$4</f>
             </numRef>
           </val>
         </ser>
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -834,8 +834,55 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-08-18 20:32:52</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D5">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -855,7 +902,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G4">
+  <conditionalFormatting sqref="G2:G5">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -863,17 +910,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H4">
+  <conditionalFormatting sqref="H2:H5">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I4">
+  <conditionalFormatting sqref="I2:I5">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J4">
+  <conditionalFormatting sqref="J2:J5">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -888,7 +935,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -928,6 +975,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 20:42:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -881,8 +881,60 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Fout bij verwerken (forward_to_fallback() got an unexpected keyword argument 'afzender')</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-08-18 20:42:03</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -902,7 +954,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -910,17 +962,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="J2:J6">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -972,7 +1024,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 20:48:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -933,8 +933,60 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Interne taak</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>kwaliteit@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Leg dit even neer bij Koen.</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Fout bij verwerken (forward_to_fallback() got an unexpected keyword argument 'fallback_email')</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-08-18 20:48:17</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D6">
+  <conditionalFormatting sqref="D2:D7">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -954,7 +1006,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G6">
+  <conditionalFormatting sqref="G2:G7">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -962,17 +1014,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H6">
+  <conditionalFormatting sqref="H2:H7">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I6">
+  <conditionalFormatting sqref="I2:I7">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J6">
+  <conditionalFormatting sqref="J2:J7">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1010,17 +1062,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Onbekend</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Onbekend</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 20:56:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -985,8 +985,50 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Geen onderwerp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>onbekend</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-08-18 20:56:03</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D7">
+  <conditionalFormatting sqref="D2:D8">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1006,7 +1048,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G7">
+  <conditionalFormatting sqref="G2:G8">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1014,17 +1056,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H7">
+  <conditionalFormatting sqref="H2:H8">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I7">
+  <conditionalFormatting sqref="I2:I8">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J7">
+  <conditionalFormatting sqref="J2:J8">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1066,7 +1108,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 21:12:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1027,8 +1027,42 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Geen onderwerp</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>onbekend</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-08-18 21:12:41</t>
+        </is>
+      </c>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D8">
+  <conditionalFormatting sqref="D2:D9">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1048,7 +1082,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8">
+  <conditionalFormatting sqref="G2:G9">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1056,17 +1090,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H8">
+  <conditionalFormatting sqref="H2:H9">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I9">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J8">
+  <conditionalFormatting sqref="J2:J9">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1128,7 +1162,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 21:21:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1061,8 +1061,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Geen onderwerp</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>onbekend</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-08-18 21:20:52</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D9">
+  <conditionalFormatting sqref="D2:D10">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1082,7 +1124,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9">
+  <conditionalFormatting sqref="G2:G10">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1090,17 +1132,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H9">
+  <conditionalFormatting sqref="H2:H10">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I9">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J9">
+  <conditionalFormatting sqref="J2:J10">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1142,7 +1184,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 21:25:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,8 +1103,50 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Geen onderwerp</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>onbekend</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-08-18 21:25:44</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D2:D11">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1124,7 +1166,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10">
+  <conditionalFormatting sqref="G2:G11">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1132,17 +1174,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H10">
+  <conditionalFormatting sqref="H2:H11">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I10">
+  <conditionalFormatting sqref="I2:I11">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J10">
+  <conditionalFormatting sqref="J2:J11">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1190,17 +1232,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Intern verzoek / Actie voor medewerker</t>
+          <t>Overig</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Overig</t>
+          <t>Intern verzoek / Actie voor medewerker</t>
         </is>
       </c>
       <c r="B4" t="n">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 21:35:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1145,8 +1145,50 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Geen onderwerp</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>onbekend</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-08-18 21:35:03</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D11">
+  <conditionalFormatting sqref="D2:D12">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1166,7 +1208,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G11">
+  <conditionalFormatting sqref="G2:G12">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1174,17 +1216,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H11">
+  <conditionalFormatting sqref="H2:H12">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I11">
+  <conditionalFormatting sqref="I2:I12">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J11">
+  <conditionalFormatting sqref="J2:J12">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1236,7 +1278,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Automatische test-sync: 2025-08-18 21:41:50
</commit_message>
<xml_diff>
--- a/logs/mail_log_2025-08-18.xlsx
+++ b/logs/mail_log_2025-08-18.xlsx
@@ -623,7 +623,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1187,8 +1187,50 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Geen onderwerp</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>no-reply@testbedrijf123.nl</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-08-18 21:40:55</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D12">
+  <conditionalFormatting sqref="D2:D13">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0">
       <formula>"Klacht"</formula>
     </cfRule>
@@ -1208,7 +1250,7 @@
       <formula>"Overig"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G12">
+  <conditionalFormatting sqref="G2:G13">
     <cfRule type="cellIs" priority="7" operator="equal" dxfId="2">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1216,17 +1258,17 @@
       <formula>"Nee"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" priority="9" operator="equal" dxfId="5">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="I2:I13">
     <cfRule type="cellIs" priority="10" operator="equal" dxfId="6">
       <formula>"Ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J12">
+  <conditionalFormatting sqref="J2:J13">
     <cfRule type="cellIs" priority="11" operator="equal" dxfId="7">
       <formula>"Ja"</formula>
     </cfRule>
@@ -1278,7 +1320,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">

</xml_diff>